<commit_message>
doc: Updated with full test run
</commit_message>
<xml_diff>
--- a/Csharp_Algorithms_lists/Doc/PerformanceAnalysis.xlsx
+++ b/Csharp_Algorithms_lists/Doc/PerformanceAnalysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\CSharp\Algorithms in C#\Csharp_Algorithms_lists\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{955F8646-A713-422F-A097-37147679A545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21159ACF-4574-45A3-8F92-E6AA156BDE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12225" yWindow="3855" windowWidth="38700" windowHeight="15435" xr2:uid="{6A0CDCAA-BC5F-4CE4-85A0-0C63848EA4D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Visualization" sheetId="2" r:id="rId1"/>
+    <sheet name="TestReport" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="51">
   <si>
     <t>timestamp</t>
   </si>
@@ -120,9 +121,6 @@
     <t>name11</t>
   </si>
   <si>
-    <t>01/23/2022 13:27:15</t>
-  </si>
-  <si>
     <t>D:\src\CSharp\Algorithms in C#\Csharp_Algorithms_lists\Test\CSharp_Algorithms_lists_Tests\bin\Debug\net6.0\CSharp_Algorithms_lists_Tests.dll</t>
   </si>
   <si>
@@ -186,9 +184,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Skip</t>
-  </si>
-  <si>
     <t>TestType</t>
   </si>
   <si>
@@ -198,7 +193,7 @@
     <t>DictionaryBased</t>
   </si>
   <si>
-    <t>LongRunning</t>
+    <t>01/23/2022 13:35:37</t>
   </si>
 </sst>
 </file>
@@ -363,7 +358,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ark1'!$X$2</c:f>
+              <c:f>TestReport!$X$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -386,24 +381,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$U$2:$U$7</c:f>
+              <c:f>TestReport!$U$2:$U$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.1790000000000001E-2</c:v>
+                  <c:v>3.7335800000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16237019999999999</c:v>
+                  <c:v>0.1500417</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55333759999999999</c:v>
+                  <c:v>0.55572169999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.0256311</c:v>
+                  <c:v>11.7304023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.840091999999999</c:v>
+                  <c:v>46.085132299999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1159.9982726000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5507.6066547</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -411,7 +412,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9B74-45E0-A423-9BD96E5B153C}"/>
+              <c16:uniqueId val="{00000000-C2D1-4520-AC3D-3931BE7C84C1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -420,7 +421,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ark1'!$X$10</c:f>
+              <c:f>TestReport!$X$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -443,24 +444,30 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$U$10:$U$15</c:f>
+              <c:f>TestReport!$U$9:$U$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.3102000000000002E-3</c:v>
+                  <c:v>6.9736300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.13842E-2</c:v>
+                  <c:v>8.7879499999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21481539999999999</c:v>
+                  <c:v>0.1549343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59180560000000004</c:v>
+                  <c:v>1.9300322999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6634049</c:v>
+                  <c:v>1.9333441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.2842409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.170217399999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,7 +475,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9B74-45E0-A423-9BD96E5B153C}"/>
+              <c16:uniqueId val="{00000001-C2D1-4520-AC3D-3931BE7C84C1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -491,6 +498,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -634,11 +642,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1198,31 +1201,34 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{51266DB5-3F1C-4B23-BC27-38AEDDB10A20}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>4848225</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9298983" cy="6078242"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A354AFC-4468-4D05-9AFB-228B2B9C6D14}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DC82A6-A03B-4D1B-BF39-75DF558A71E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1235,21 +1241,15 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E53D15A3-2715-4796-BC2F-849698EF2EB7}" name="Tabel1" displayName="Tabel1" ref="A1:Z15" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:Z15" xr:uid="{E53D15A3-2715-4796-BC2F-849698EF2EB7}">
-    <filterColumn colId="21">
-      <filters>
-        <filter val="Pass"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z15">
-    <sortCondition ref="X1:X15"/>
+  <autoFilter ref="A1:Z15" xr:uid="{E53D15A3-2715-4796-BC2F-849698EF2EB7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:Z15">
+    <sortCondition ref="U1:U15"/>
   </sortState>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{69764B4A-C562-412C-8D6E-D5FF5D5A6223}" uniqueName="timestamp" name="timestamp">
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29203674-E54A-433C-86F9-DE580105733D}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1648,7 @@
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -1656,15 +1656,15 @@
     <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="65.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1749,31 +1749,31 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C2" s="2">
         <v>44584</v>
       </c>
       <c r="D2" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E2">
         <v>14</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1783,71 +1783,71 @@
         <v>7</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2">
+        <v>3.7335800000000002E-2</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U2">
-        <v>4.1790000000000001E-2</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="X2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>44584</v>
       </c>
       <c r="D3" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E3">
         <v>14</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1857,75 +1857,71 @@
         <v>7</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q3">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3">
+        <v>0.1500417</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U3">
-        <v>1E-3</v>
-      </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>44584</v>
       </c>
       <c r="D4" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E4">
         <v>14</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1935,71 +1931,71 @@
         <v>7</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q4">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4">
+        <v>0.55572169999999999</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U4">
-        <v>0.16237019999999999</v>
-      </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="X4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C5" s="2">
         <v>44584</v>
       </c>
       <c r="D5" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E5">
         <v>14</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2009,71 +2005,71 @@
         <v>7</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q5">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5">
+        <v>11.7304023</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U5">
-        <v>0.55333759999999999</v>
-      </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="X5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C6" s="2">
         <v>44584</v>
       </c>
       <c r="D6" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E6">
         <v>14</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -2083,71 +2079,71 @@
         <v>7</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q6">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6">
+        <v>46.085132299999998</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U6">
-        <v>13.0256311</v>
-      </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="X6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="2">
         <v>44584</v>
       </c>
       <c r="D7" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E7">
         <v>14</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -2157,71 +2153,71 @@
         <v>7</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q7">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7">
+        <v>1159.9982726000001</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U7">
-        <v>45.840091999999999</v>
-      </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="X7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C8" s="2">
         <v>44584</v>
       </c>
       <c r="D8" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E8">
         <v>14</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2231,75 +2227,71 @@
         <v>7</v>
       </c>
       <c r="M8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q8">
-        <v>59.625</v>
+        <v>6726.1639999999998</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8">
+        <v>5507.6066547</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U8">
-        <v>1E-3</v>
-      </c>
-      <c r="V8" s="1" t="s">
+      <c r="W8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X8" s="1" t="s">
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z8" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C9" s="2">
         <v>44584</v>
       </c>
       <c r="D9" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E9">
         <v>14</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2309,75 +2301,71 @@
         <v>7</v>
       </c>
       <c r="M9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q9">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9">
+        <v>6.9736300000000001E-2</v>
+      </c>
+      <c r="V9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U9">
-        <v>1E-3</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="W9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C10" s="2">
         <v>44584</v>
       </c>
       <c r="D10" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E10">
         <v>14</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2387,71 +2375,71 @@
         <v>7</v>
       </c>
       <c r="M10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
       <c r="O10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q10">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10">
+        <v>8.7879499999999999E-2</v>
+      </c>
+      <c r="V10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U10">
-        <v>6.3102000000000002E-3</v>
-      </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C11" s="2">
         <v>44584</v>
       </c>
       <c r="D11" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E11">
         <v>14</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2461,71 +2449,71 @@
         <v>7</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q11">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="U11">
+        <v>0.1549343</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U11">
-        <v>6.13842E-2</v>
-      </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C12" s="2">
         <v>44584</v>
       </c>
       <c r="D12" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E12">
         <v>14</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2535,71 +2523,71 @@
         <v>7</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q12">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="U12">
+        <v>1.9300322999999999</v>
+      </c>
+      <c r="V12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U12">
-        <v>0.21481539999999999</v>
-      </c>
-      <c r="V12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C13" s="2">
         <v>44584</v>
       </c>
       <c r="D13" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E13">
         <v>14</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2609,71 +2597,71 @@
         <v>7</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q13">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="U13">
+        <v>1.9333441</v>
+      </c>
+      <c r="V13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U13">
-        <v>0.59180560000000004</v>
-      </c>
-      <c r="V13" s="1" t="s">
+      <c r="W13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C14" s="2">
         <v>44584</v>
       </c>
       <c r="D14" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E14">
         <v>14</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -2683,75 +2671,71 @@
         <v>7</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q14">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="U14">
+        <v>12.2842409</v>
+      </c>
+      <c r="V14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U14">
-        <v>1E-3</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="W14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C15" s="2">
         <v>44584</v>
       </c>
       <c r="D15" s="3">
-        <v>0.56059027777777781</v>
+        <v>0.56640046296296298</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>60.402999999999999</v>
+        <v>6727.0290000000005</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2761,49 +2745,48 @@
         <v>7</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q15">
-        <v>2.54</v>
+        <v>33.630000000000003</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="U15">
+        <v>17.170217399999999</v>
+      </c>
+      <c r="V15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U15">
-        <v>1.6634049</v>
-      </c>
-      <c r="V15" s="1" t="s">
+      <c r="W15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
doc: updated readme files
</commit_message>
<xml_diff>
--- a/Csharp_Algorithms_lists/Doc/PerformanceAnalysis.xlsx
+++ b/Csharp_Algorithms_lists/Doc/PerformanceAnalysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\CSharp\Algorithms in C#\Csharp_Algorithms_lists\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21159ACF-4574-45A3-8F92-E6AA156BDE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C353A182-6986-4502-B83E-AC1460139B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12225" yWindow="3855" windowWidth="38700" windowHeight="15435" xr2:uid="{6A0CDCAA-BC5F-4CE4-85A0-0C63848EA4D1}"/>
+    <workbookView xWindow="11550" yWindow="3810" windowWidth="38700" windowHeight="15345" xr2:uid="{6A0CDCAA-BC5F-4CE4-85A0-0C63848EA4D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Visualization" sheetId="2" r:id="rId1"/>
-    <sheet name="TestReport" sheetId="1" r:id="rId2"/>
+    <sheet name="TestReport" sheetId="1" r:id="rId1"/>
+    <sheet name="Visualization" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -324,6 +324,612 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Array</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TestReport!$U$2:$U$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.7335800000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1500417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55572169999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.7304023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.085132299999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E968-4CD5-9841-3D3749759118}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Dictionary</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TestReport!$U$9:$U$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.9736300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7879499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1549343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9300322999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9333441</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E968-4CD5-9841-3D3749759118}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="783990400"/>
+        <c:axId val="783979584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="783990400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="783979584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="783979584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="783990400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Arrays</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TestReport!$U$2:$U$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.7335800000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1500417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55572169999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.7304023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.085132299999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1159.9982726000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5507.6066547</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-5114-4A3B-866A-658CB0B6017A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Dictionary</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TestReport!$U$9:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9736300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7879499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1549343</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9300322999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9333441</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.2842409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.170217399999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-5114-4A3B-866A-658CB0B6017A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="783990400"/>
+        <c:axId val="783979584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="783990400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="783979584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="783979584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="783990400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
@@ -532,7 +1138,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1672921727"/>
@@ -591,7 +1197,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1672912159"/>
@@ -639,7 +1245,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -685,6 +1291,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1201,11 +1847,527 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{51266DB5-3F1C-4B23-BC27-38AEDDB10A20}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1214,9 +2376,86 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D47248F-D8DF-4040-AE37-3BCA848FFF9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>5324475</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE417AC8-BEC5-450F-A11B-93E0B51F402F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298983" cy="6078242"/>
+    <xdr:ext cx="9297051" cy="6073205"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1">
@@ -1634,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29203674-E54A-433C-86F9-DE580105733D}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +2896,7 @@
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="65.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="109.85546875" customWidth="1"/>
     <col min="19" max="19" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
@@ -2785,8 +4024,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>